<commit_message>
add user input params table
</commit_message>
<xml_diff>
--- a/Notes_and_Guides/METR_Tables.xlsx
+++ b/Notes_and_Guides/METR_Tables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Complex Parameters" sheetId="2" r:id="rId2"/>
     <sheet name="All" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="102">
   <si>
     <t>Parameter</t>
   </si>
@@ -312,6 +313,21 @@
   </si>
   <si>
     <t>Statutory business entity-level income tax</t>
+  </si>
+  <si>
+    <t>User Defined Parameters</t>
+  </si>
+  <si>
+    <t>Haircut to Interest Deduction</t>
+  </si>
+  <si>
+    <t>Allowance for Corporate Equity</t>
+  </si>
+  <si>
+    <t>Notation?</t>
+  </si>
+  <si>
+    <t>User Input</t>
   </si>
 </sst>
 </file>
@@ -372,7 +388,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -395,6 +411,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -402,7 +422,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -420,6 +440,10 @@
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -922,7 +946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -1403,7 +1427,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A18" sqref="A18:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1966,4 +1990,313 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="CBO Economic Forecast"/>
+    <hyperlink ref="C4" r:id="rId2" display="CBO Economic Forecast"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add user defined params
</commit_message>
<xml_diff>
--- a/Notes_and_Guides/METR_Tables.xlsx
+++ b/Notes_and_Guides/METR_Tables.xlsx
@@ -1997,7 +1997,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2092,7 +2092,7 @@
         <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>

</xml_diff>